<commit_message>
Found error in spring reference and fixed. Changed current springs constant to 3 to increase responsiveness. removed old files. removed gif creation to speed up sim.
</commit_message>
<xml_diff>
--- a/Mass-model/Mass model/Springs.xlsx
+++ b/Mass-model/Mass model/Springs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{A997774F-8F07-4FEC-890F-36A636A06BD8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{7F81EADF-8B81-4BD1-95E0-CB45416CDB30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE97340-67C8-40E9-99AE-0B91345A71A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE4D78-414E-44D6-B24F-75CEDEE78EE4}">
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>